<commit_message>
added comment to the pcc graphic
</commit_message>
<xml_diff>
--- a/PCC.xlsx
+++ b/PCC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simone Benedetti\Documents\MEGA\ISW2\Process Control Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simone Benedetti\Documents\Programmazione JAVA\ProcessControlChart\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B679BF-F40B-4A0C-B77E-DF0230DB185B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B01AA26-ADFF-4E98-8261-794FE1E832A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7E45DBF2-D3E5-4B39-ADB1-550BA4683CEA}"/>
   </bookViews>
@@ -250,11 +250,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2533,7 +2534,86 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CasellaDiTesto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD34CA63-374D-4B5D-A34B-1C7A753D2CCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915150" y="5288280"/>
+          <a:ext cx="4815840" cy="834390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100"/>
+            <a:t>Il grafico</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" baseline="0"/>
+            <a:t> mostra che il numero maggiore di commit riguardanti nuove Feature del progetto "Bahir" sono state effettuate ad Agosto 2016 e a Marzo 2017. Non ci sono punti al di fuori delle rette limite quindi non c'è stato un numero di nuove Feature considerevole nel periodo preso in considerazione.</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2835,8 +2915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991724A8-5DAF-4DEF-A326-CCC81EFB5CF9}">
   <dimension ref="B4:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2866,7 +2946,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D28" si="0">Upper_limit</f>
+        <f t="shared" ref="D5:D27" si="0">Upper_limit</f>
         <v>3.5980760876827937</v>
       </c>
       <c r="E5">
@@ -2903,7 +2983,7 @@
         <v>3.5980760876827937</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E28" si="1">$E$5</f>
+        <f t="shared" ref="E7:E27" si="1">$E$5</f>
         <v>1.3846153846153846</v>
       </c>
       <c r="F7">
@@ -3281,7 +3361,7 @@
         <v>31</v>
       </c>
       <c r="D28">
-        <f>Upper_limit</f>
+        <f t="shared" ref="D28:D52" si="3">Upper_limit</f>
         <v>3.5980760876827937</v>
       </c>
       <c r="E28">
@@ -3298,11 +3378,11 @@
         <v>32</v>
       </c>
       <c r="D29">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E29">
-        <f t="shared" ref="E29:E52" si="3">$E$5</f>
+        <f t="shared" ref="E29:E52" si="4">$E$5</f>
         <v>1.3846153846153846</v>
       </c>
       <c r="F29">
@@ -3314,11 +3394,11 @@
         <v>33</v>
       </c>
       <c r="D30">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F30">
@@ -3337,11 +3417,11 @@
         <v>34</v>
       </c>
       <c r="D31">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F31">
@@ -3360,11 +3440,11 @@
         <v>35</v>
       </c>
       <c r="D32">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F32">
@@ -3372,16 +3452,16 @@
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D33">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F33">
@@ -3395,16 +3475,16 @@
         <v>3.5980760876827937</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D34">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F34">
@@ -3418,7 +3498,7 @@
         <v>-0.82884531845202458</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
@@ -3426,66 +3506,67 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D36">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D37">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D38">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
@@ -3493,18 +3574,18 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
@@ -3512,98 +3593,98 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D41">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D42">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D43">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D44">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D45">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="1" t="s">
         <v>49</v>
       </c>
@@ -3611,43 +3692,43 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D47">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D48">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F48">
@@ -3659,11 +3740,11 @@
         <v>52</v>
       </c>
       <c r="D49">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F49">
@@ -3675,11 +3756,11 @@
         <v>53</v>
       </c>
       <c r="D50">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F50">
@@ -3691,11 +3772,11 @@
         <v>54</v>
       </c>
       <c r="D51">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F51">
@@ -3710,11 +3791,11 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <f>Upper_limit</f>
+        <f t="shared" si="3"/>
         <v>3.5980760876827937</v>
       </c>
       <c r="E52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3846153846153846</v>
       </c>
       <c r="F52">

</xml_diff>